<commit_message>
fix - index 설정 오류 수정
</commit_message>
<xml_diff>
--- a/opendata-crawler/testOutput.xlsx
+++ b/opendata-crawler/testOutput.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,64 +424,64 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>고용노동부_사업체노동력조사</t>
+          <t>데이터 제목</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>사업체의 종사자수, 빈 일자리, 노동이동, 근로시간, 임금 등에 관한 사항을 정기적으로 조사하여 산업 유형별 고용상황과 근로시간, 임금상승률 등에 관한 지표를 제공</t>
+          <t>상세설명</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>https://www.data.go.kr/data/3038232/fileData.do</t>
+          <t>바로가기 링크</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>고용노동부</t>
+          <t>제공기관</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>2023-03-31</t>
+          <t>수정일</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>4879</t>
+          <t>조회수</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>1836</t>
+          <t>다운로드</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>주기성 데이터</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>근로자수,빈일자리수,임금</t>
+          <t>키워드</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>고용노동부_사업체노동력조사</t>
+          <t>고용노동부_신규화학물질</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>사업체의 종사자수, 빈 일자리, 노동이동, 근로시간, 임금 등에 관한 사항을 정기적으로 조사하여 산업 유형별 고용상황과 근로시간, 임금상승률 등에 관한 지표를 제공</t>
+          <t>고용노동부가 공표한 신규화학물질의 명칭, 유해성, 제조 수입량, 위험성 정보, 근로자 건강장해 예방을 위한 조치사항 제공</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://www.data.go.kr/data/3038232/fileData.do</t>
+          <t>https://www.data.go.kr/data/15002450/fileData.do</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -491,44 +491,44 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2023-03-31</t>
+          <t>2023-04-13</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>4879</t>
+          <t>3480</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>1836</t>
+          <t>1414</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>10</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>근로자수,빈일자리수,임금</t>
+          <t>화학물질,유해성,위험성</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>고용노동부_사업체노동력조사</t>
+          <t>고용노동부_근로자 건강센터 현황</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>사업체의 종사자수, 빈 일자리, 노동이동, 근로시간, 임금 등에 관한 사항을 정기적으로 조사하여 산업 유형별 고용상황과 근로시간, 임금상승률 등에 관한 지표를 제공</t>
+          <t>보건관리가 취약한 소규모 사업장 근로자의 직업병예방 및 건강증진을 위한 기초 직업건강서비스를 제공하기 위해 설치한 근로자 건강센터 설치현황</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://www.data.go.kr/data/3038232/fileData.do</t>
+          <t>https://www.data.go.kr/data/15002433/fileData.do</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -538,44 +538,44 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2023-03-31</t>
+          <t>2023-04-06</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>4879</t>
+          <t>3056</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>1836</t>
+          <t>943</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>근로자수,빈일자리수,임금</t>
+          <t>건강센터,건강지원센터,센터</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>고용노동부_사업체노동력조사</t>
+          <t>고용노동부_건설재해예방전문지도기관</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>사업체의 종사자수, 빈 일자리, 노동이동, 근로시간, 임금 등에 관한 사항을 정기적으로 조사하여 산업 유형별 고용상황과 근로시간, 임금상승률 등에 관한 지표를 제공</t>
+          <t>고용노동부가 공표한 건설재해예방전문지도기관 명단으로 지도기관명, 주소, 전화번호, 관할 지방관서, 지도분야 등에 대한 정보를 제공합니다.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://www.data.go.kr/data/3038232/fileData.do</t>
+          <t>https://www.data.go.kr/data/15113114/fileData.do</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -585,44 +585,39 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2023-03-31</t>
+          <t>2023-04-06</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>4879</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>1836</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>14</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>근로자수,빈일자리수,임금</t>
+          <t>건설안전,기술지도,건설재해예방</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>고용노동부_사업체노동력조사</t>
+          <t>고용노동부_일가정양립실태조사 보고서</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>사업체의 종사자수, 빈 일자리, 노동이동, 근로시간, 임금 등에 관한 사항을 정기적으로 조사하여 산업 유형별 고용상황과 근로시간, 임금상승률 등에 관한 지표를 제공</t>
+          <t>매년 한국여성정책연구원에 연구용역을 의뢰하여 작성한 연구보고서일가정 양립을 위한 모성보호, 유연근로 실태 현황조사에 대한 보고서</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://www.data.go.kr/data/3038232/fileData.do</t>
+          <t>https://www.data.go.kr/data/15032836/fileData.do</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -632,27 +627,27 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2023-03-31</t>
+          <t>2023-04-04</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>4879</t>
+          <t>3853</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>1836</t>
+          <t>608</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>근로자수,빈일자리수,임금</t>
+          <t>모성보호,유연근로,일가정양립</t>
         </is>
       </c>
     </row>
@@ -706,17 +701,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>고용노동부_사업체노동력조사</t>
+          <t>고용노동부_신규화학물질</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>사업체의 종사자수, 빈 일자리, 노동이동, 근로시간, 임금 등에 관한 사항을 정기적으로 조사하여 산업 유형별 고용상황과 근로시간, 임금상승률 등에 관한 지표를 제공</t>
+          <t>고용노동부가 공표한 신규화학물질의 명칭, 유해성, 제조 수입량, 위험성 정보, 근로자 건강장해 예방을 위한 조치사항 제공</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://www.data.go.kr/data/3038232/fileData.do</t>
+          <t>https://www.data.go.kr/data/15002450/fileData.do</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -726,44 +721,44 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2023-03-31</t>
+          <t>2023-04-13</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>4879</t>
+          <t>3480</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>1836</t>
+          <t>1414</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>10</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>근로자수,빈일자리수,임금</t>
+          <t>화학물질,유해성,위험성</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>고용노동부_사업체노동력조사</t>
+          <t>고용노동부_근로자 건강센터 현황</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>사업체의 종사자수, 빈 일자리, 노동이동, 근로시간, 임금 등에 관한 사항을 정기적으로 조사하여 산업 유형별 고용상황과 근로시간, 임금상승률 등에 관한 지표를 제공</t>
+          <t>보건관리가 취약한 소규모 사업장 근로자의 직업병예방 및 건강증진을 위한 기초 직업건강서비스를 제공하기 위해 설치한 근로자 건강센터 설치현황</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://www.data.go.kr/data/3038232/fileData.do</t>
+          <t>https://www.data.go.kr/data/15002433/fileData.do</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -773,44 +768,44 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2023-03-31</t>
+          <t>2023-04-06</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>4879</t>
+          <t>3056</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>1836</t>
+          <t>943</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>근로자수,빈일자리수,임금</t>
+          <t>건강센터,건강지원센터,센터</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>고용노동부_사업체노동력조사</t>
+          <t>고용노동부_건설재해예방전문지도기관</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>사업체의 종사자수, 빈 일자리, 노동이동, 근로시간, 임금 등에 관한 사항을 정기적으로 조사하여 산업 유형별 고용상황과 근로시간, 임금상승률 등에 관한 지표를 제공</t>
+          <t>고용노동부가 공표한 건설재해예방전문지도기관 명단으로 지도기관명, 주소, 전화번호, 관할 지방관서, 지도분야 등에 대한 정보를 제공합니다.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://www.data.go.kr/data/3038232/fileData.do</t>
+          <t>https://www.data.go.kr/data/15113114/fileData.do</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -820,44 +815,39 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2023-03-31</t>
+          <t>2023-04-06</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>4879</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>1836</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>14</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>근로자수,빈일자리수,임금</t>
+          <t>건설안전,기술지도,건설재해예방</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>고용노동부_사업체노동력조사</t>
+          <t>고용노동부_일가정양립실태조사 보고서</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>사업체의 종사자수, 빈 일자리, 노동이동, 근로시간, 임금 등에 관한 사항을 정기적으로 조사하여 산업 유형별 고용상황과 근로시간, 임금상승률 등에 관한 지표를 제공</t>
+          <t>매년 한국여성정책연구원에 연구용역을 의뢰하여 작성한 연구보고서일가정 양립을 위한 모성보호, 유연근로 실태 현황조사에 대한 보고서</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://www.data.go.kr/data/3038232/fileData.do</t>
+          <t>https://www.data.go.kr/data/15032836/fileData.do</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -867,27 +857,27 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2023-03-31</t>
+          <t>2023-04-04</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>4879</t>
+          <t>3853</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>1836</t>
+          <t>608</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>근로자수,빈일자리수,임금</t>
+          <t>모성보호,유연근로,일가정양립</t>
         </is>
       </c>
     </row>
@@ -941,17 +931,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>고용노동부_사업체노동력조사</t>
+          <t>고용노동부_신규화학물질</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>사업체의 종사자수, 빈 일자리, 노동이동, 근로시간, 임금 등에 관한 사항을 정기적으로 조사하여 산업 유형별 고용상황과 근로시간, 임금상승률 등에 관한 지표를 제공</t>
+          <t>고용노동부가 공표한 신규화학물질의 명칭, 유해성, 제조 수입량, 위험성 정보, 근로자 건강장해 예방을 위한 조치사항 제공</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://www.data.go.kr/data/3038232/fileData.do</t>
+          <t>https://www.data.go.kr/data/15002450/fileData.do</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -961,44 +951,44 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2023-03-31</t>
+          <t>2023-04-13</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>4879</t>
+          <t>3480</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>1836</t>
+          <t>1414</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>10</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>근로자수,빈일자리수,임금</t>
+          <t>화학물질,유해성,위험성</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>고용노동부_사업체노동력조사</t>
+          <t>고용노동부_근로자 건강센터 현황</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>사업체의 종사자수, 빈 일자리, 노동이동, 근로시간, 임금 등에 관한 사항을 정기적으로 조사하여 산업 유형별 고용상황과 근로시간, 임금상승률 등에 관한 지표를 제공</t>
+          <t>보건관리가 취약한 소규모 사업장 근로자의 직업병예방 및 건강증진을 위한 기초 직업건강서비스를 제공하기 위해 설치한 근로자 건강센터 설치현황</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://www.data.go.kr/data/3038232/fileData.do</t>
+          <t>https://www.data.go.kr/data/15002433/fileData.do</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1008,44 +998,44 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2023-03-31</t>
+          <t>2023-04-06</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>4879</t>
+          <t>3056</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>1836</t>
+          <t>943</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>근로자수,빈일자리수,임금</t>
+          <t>건강센터,건강지원센터,센터</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>고용노동부_사업체노동력조사</t>
+          <t>고용노동부_건설재해예방전문지도기관</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>사업체의 종사자수, 빈 일자리, 노동이동, 근로시간, 임금 등에 관한 사항을 정기적으로 조사하여 산업 유형별 고용상황과 근로시간, 임금상승률 등에 관한 지표를 제공</t>
+          <t>고용노동부가 공표한 건설재해예방전문지도기관 명단으로 지도기관명, 주소, 전화번호, 관할 지방관서, 지도분야 등에 대한 정보를 제공합니다.</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://www.data.go.kr/data/3038232/fileData.do</t>
+          <t>https://www.data.go.kr/data/15113114/fileData.do</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1055,44 +1045,39 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2023-03-31</t>
+          <t>2023-04-06</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>4879</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>1836</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>14</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>근로자수,빈일자리수,임금</t>
+          <t>건설안전,기술지도,건설재해예방</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>고용노동부_사업체노동력조사</t>
+          <t>고용노동부_일가정양립실태조사 보고서</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>사업체의 종사자수, 빈 일자리, 노동이동, 근로시간, 임금 등에 관한 사항을 정기적으로 조사하여 산업 유형별 고용상황과 근로시간, 임금상승률 등에 관한 지표를 제공</t>
+          <t>매년 한국여성정책연구원에 연구용역을 의뢰하여 작성한 연구보고서일가정 양립을 위한 모성보호, 유연근로 실태 현황조사에 대한 보고서</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://www.data.go.kr/data/3038232/fileData.do</t>
+          <t>https://www.data.go.kr/data/15032836/fileData.do</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1102,27 +1087,27 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2023-03-31</t>
+          <t>2023-04-04</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>4879</t>
+          <t>3853</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>1836</t>
+          <t>608</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>근로자수,빈일자리수,임금</t>
+          <t>모성보호,유연근로,일가정양립</t>
         </is>
       </c>
     </row>
@@ -1176,17 +1161,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>고용노동부_사업체노동력조사</t>
+          <t>고용노동부_신규화학물질</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>사업체의 종사자수, 빈 일자리, 노동이동, 근로시간, 임금 등에 관한 사항을 정기적으로 조사하여 산업 유형별 고용상황과 근로시간, 임금상승률 등에 관한 지표를 제공</t>
+          <t>고용노동부가 공표한 신규화학물질의 명칭, 유해성, 제조 수입량, 위험성 정보, 근로자 건강장해 예방을 위한 조치사항 제공</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://www.data.go.kr/data/3038232/fileData.do</t>
+          <t>https://www.data.go.kr/data/15002450/fileData.do</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1196,72 +1181,3428 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2023-03-31</t>
+          <t>2023-04-13</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>4879</t>
+          <t>3480</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>1836</t>
+          <t>1414</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>10</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>근로자수,빈일자리수,임금</t>
+          <t>화학물질,유해성,위험성</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>고용노동부_근로자 건강센터 현황</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>보건관리가 취약한 소규모 사업장 근로자의 직업병예방 및 건강증진을 위한 기초 직업건강서비스를 제공하기 위해 설치한 근로자 건강센터 설치현황</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15002433/fileData.do</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2023-04-06</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>3056</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>943</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>건강센터,건강지원센터,센터</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>고용노동부_건설재해예방전문지도기관</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>고용노동부가 공표한 건설재해예방전문지도기관 명단으로 지도기관명, 주소, 전화번호, 관할 지방관서, 지도분야 등에 대한 정보를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15113114/fileData.do</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2023-04-06</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>건설안전,기술지도,건설재해예방</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>고용노동부_일가정양립실태조사 보고서</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>매년 한국여성정책연구원에 연구용역을 의뢰하여 작성한 연구보고서일가정 양립을 위한 모성보호, 유연근로 실태 현황조사에 대한 보고서</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15032836/fileData.do</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2023-04-04</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>3853</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>608</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>모성보호,유연근로,일가정양립</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
           <t>고용노동부_사업체노동력조사</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B21" t="inlineStr">
         <is>
           <t>사업체의 종사자수, 빈 일자리, 노동이동, 근로시간, 임금 등에 관한 사항을 정기적으로 조사하여 산업 유형별 고용상황과 근로시간, 임금상승률 등에 관한 지표를 제공</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>https://www.data.go.kr/data/3038232/fileData.do</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>고용노동부</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
         <is>
           <t>2023-03-31</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="F21" t="inlineStr">
         <is>
           <t>4879</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="G21" t="inlineStr">
         <is>
           <t>1836</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
+      <c r="H21" t="inlineStr">
         <is>
           <t>14</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr">
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>근로자수,빈일자리수,임금</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>고용노동부_신규화학물질</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>고용노동부가 공표한 신규화학물질의 명칭, 유해성, 제조 수입량, 위험성 정보, 근로자 건강장해 예방을 위한 조치사항 제공</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15002450/fileData.do</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>2023-04-13</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>3480</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>1414</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>화학물질,유해성,위험성</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>고용노동부_근로자 건강센터 현황</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>보건관리가 취약한 소규모 사업장 근로자의 직업병예방 및 건강증진을 위한 기초 직업건강서비스를 제공하기 위해 설치한 근로자 건강센터 설치현황</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15002433/fileData.do</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>2023-04-06</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>3056</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>943</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>건강센터,건강지원센터,센터</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>고용노동부_건설재해예방전문지도기관</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>고용노동부가 공표한 건설재해예방전문지도기관 명단으로 지도기관명, 주소, 전화번호, 관할 지방관서, 지도분야 등에 대한 정보를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15113114/fileData.do</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>2023-04-06</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>건설안전,기술지도,건설재해예방</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>고용노동부_일가정양립실태조사 보고서</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>매년 한국여성정책연구원에 연구용역을 의뢰하여 작성한 연구보고서일가정 양립을 위한 모성보호, 유연근로 실태 현황조사에 대한 보고서</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15032836/fileData.do</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>2023-04-04</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>3853</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>608</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>모성보호,유연근로,일가정양립</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>고용노동부_사업체노동력조사</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>사업체의 종사자수, 빈 일자리, 노동이동, 근로시간, 임금 등에 관한 사항을 정기적으로 조사하여 산업 유형별 고용상황과 근로시간, 임금상승률 등에 관한 지표를 제공</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/3038232/fileData.do</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>2023-03-31</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>4879</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>1836</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>근로자수,빈일자리수,임금</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>고용노동부_신규화학물질</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>고용노동부가 공표한 신규화학물질의 명칭, 유해성, 제조 수입량, 위험성 정보, 근로자 건강장해 예방을 위한 조치사항 제공</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15002450/fileData.do</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>2023-04-13</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>3480</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>1414</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>화학물질,유해성,위험성</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>고용노동부_근로자 건강센터 현황</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>보건관리가 취약한 소규모 사업장 근로자의 직업병예방 및 건강증진을 위한 기초 직업건강서비스를 제공하기 위해 설치한 근로자 건강센터 설치현황</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15002433/fileData.do</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>2023-04-06</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>3056</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>943</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>건강센터,건강지원센터,센터</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>고용노동부_건설재해예방전문지도기관</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>고용노동부가 공표한 건설재해예방전문지도기관 명단으로 지도기관명, 주소, 전화번호, 관할 지방관서, 지도분야 등에 대한 정보를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15113114/fileData.do</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>2023-04-06</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>건설안전,기술지도,건설재해예방</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>고용노동부_일가정양립실태조사 보고서</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>매년 한국여성정책연구원에 연구용역을 의뢰하여 작성한 연구보고서일가정 양립을 위한 모성보호, 유연근로 실태 현황조사에 대한 보고서</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15032836/fileData.do</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>2023-04-04</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>3853</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>608</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>모성보호,유연근로,일가정양립</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>고용노동부_사업체노동력조사</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>사업체의 종사자수, 빈 일자리, 노동이동, 근로시간, 임금 등에 관한 사항을 정기적으로 조사하여 산업 유형별 고용상황과 근로시간, 임금상승률 등에 관한 지표를 제공</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/3038232/fileData.do</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>2023-03-31</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>4879</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>1836</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>근로자수,빈일자리수,임금</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>고용노동부_신규화학물질</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>고용노동부가 공표한 신규화학물질의 명칭, 유해성, 제조 수입량, 위험성 정보, 근로자 건강장해 예방을 위한 조치사항 제공</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15002450/fileData.do</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>2023-04-13</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>3480</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>1414</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>화학물질,유해성,위험성</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>고용노동부_근로자 건강센터 현황</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>보건관리가 취약한 소규모 사업장 근로자의 직업병예방 및 건강증진을 위한 기초 직업건강서비스를 제공하기 위해 설치한 근로자 건강센터 설치현황</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15002433/fileData.do</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>2023-04-06</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>3056</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>943</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>건강센터,건강지원센터,센터</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>고용노동부_건설재해예방전문지도기관</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>고용노동부가 공표한 건설재해예방전문지도기관 명단으로 지도기관명, 주소, 전화번호, 관할 지방관서, 지도분야 등에 대한 정보를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15113114/fileData.do</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>2023-04-06</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>건설안전,기술지도,건설재해예방</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>고용노동부_일가정양립실태조사 보고서</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>매년 한국여성정책연구원에 연구용역을 의뢰하여 작성한 연구보고서일가정 양립을 위한 모성보호, 유연근로 실태 현황조사에 대한 보고서</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15032836/fileData.do</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>2023-04-04</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>3853</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>608</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>모성보호,유연근로,일가정양립</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>고용노동부_사업체노동력조사</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>사업체의 종사자수, 빈 일자리, 노동이동, 근로시간, 임금 등에 관한 사항을 정기적으로 조사하여 산업 유형별 고용상황과 근로시간, 임금상승률 등에 관한 지표를 제공</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/3038232/fileData.do</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>2023-03-31</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>4879</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>1836</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>근로자수,빈일자리수,임금</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>고용노동부_신규화학물질</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>고용노동부가 공표한 신규화학물질의 명칭, 유해성, 제조 수입량, 위험성 정보, 근로자 건강장해 예방을 위한 조치사항 제공</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15002450/fileData.do</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>2023-04-13</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>3480</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>1414</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>화학물질,유해성,위험성</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>고용노동부_근로자 건강센터 현황</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>보건관리가 취약한 소규모 사업장 근로자의 직업병예방 및 건강증진을 위한 기초 직업건강서비스를 제공하기 위해 설치한 근로자 건강센터 설치현황</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15002433/fileData.do</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>2023-04-06</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>3056</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>943</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>건강센터,건강지원센터,센터</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>고용노동부_건설재해예방전문지도기관</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>고용노동부가 공표한 건설재해예방전문지도기관 명단으로 지도기관명, 주소, 전화번호, 관할 지방관서, 지도분야 등에 대한 정보를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15113114/fileData.do</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>2023-04-06</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>건설안전,기술지도,건설재해예방</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>고용노동부_일가정양립실태조사 보고서</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>매년 한국여성정책연구원에 연구용역을 의뢰하여 작성한 연구보고서일가정 양립을 위한 모성보호, 유연근로 실태 현황조사에 대한 보고서</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15032836/fileData.do</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>2023-04-04</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>3853</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>608</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>모성보호,유연근로,일가정양립</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>고용노동부_사업체노동력조사</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>사업체의 종사자수, 빈 일자리, 노동이동, 근로시간, 임금 등에 관한 사항을 정기적으로 조사하여 산업 유형별 고용상황과 근로시간, 임금상승률 등에 관한 지표를 제공</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/3038232/fileData.do</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>2023-03-31</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>4879</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>1836</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>근로자수,빈일자리수,임금</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>고용노동부_신규화학물질</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>고용노동부가 공표한 신규화학물질의 명칭, 유해성, 제조 수입량, 위험성 정보, 근로자 건강장해 예방을 위한 조치사항 제공</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15002450/fileData.do</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>2023-04-13</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>3480</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>1414</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>화학물질,유해성,위험성</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>고용노동부_근로자 건강센터 현황</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>보건관리가 취약한 소규모 사업장 근로자의 직업병예방 및 건강증진을 위한 기초 직업건강서비스를 제공하기 위해 설치한 근로자 건강센터 설치현황</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15002433/fileData.do</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>2023-04-06</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>3056</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>943</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>건강센터,건강지원센터,센터</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>고용노동부_건설재해예방전문지도기관</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>고용노동부가 공표한 건설재해예방전문지도기관 명단으로 지도기관명, 주소, 전화번호, 관할 지방관서, 지도분야 등에 대한 정보를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15113114/fileData.do</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>2023-04-06</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>건설안전,기술지도,건설재해예방</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>고용노동부_일가정양립실태조사 보고서</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>매년 한국여성정책연구원에 연구용역을 의뢰하여 작성한 연구보고서일가정 양립을 위한 모성보호, 유연근로 실태 현황조사에 대한 보고서</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15032836/fileData.do</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>2023-04-04</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>3853</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>608</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>모성보호,유연근로,일가정양립</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>고용노동부_사업체노동력조사</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>사업체의 종사자수, 빈 일자리, 노동이동, 근로시간, 임금 등에 관한 사항을 정기적으로 조사하여 산업 유형별 고용상황과 근로시간, 임금상승률 등에 관한 지표를 제공</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/3038232/fileData.do</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>2023-03-31</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>4879</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>1836</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>근로자수,빈일자리수,임금</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>고용노동부_신규화학물질</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>고용노동부가 공표한 신규화학물질의 명칭, 유해성, 제조 수입량, 위험성 정보, 근로자 건강장해 예방을 위한 조치사항 제공</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15002450/fileData.do</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>2023-04-13</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>3480</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>1414</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>화학물질,유해성,위험성</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>고용노동부_근로자 건강센터 현황</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>보건관리가 취약한 소규모 사업장 근로자의 직업병예방 및 건강증진을 위한 기초 직업건강서비스를 제공하기 위해 설치한 근로자 건강센터 설치현황</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15002433/fileData.do</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>2023-04-06</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>3056</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>943</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>건강센터,건강지원센터,센터</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>고용노동부_건설재해예방전문지도기관</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>고용노동부가 공표한 건설재해예방전문지도기관 명단으로 지도기관명, 주소, 전화번호, 관할 지방관서, 지도분야 등에 대한 정보를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15113114/fileData.do</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>2023-04-06</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>건설안전,기술지도,건설재해예방</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>고용노동부_일가정양립실태조사 보고서</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>매년 한국여성정책연구원에 연구용역을 의뢰하여 작성한 연구보고서일가정 양립을 위한 모성보호, 유연근로 실태 현황조사에 대한 보고서</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15032836/fileData.do</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>2023-04-04</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>3853</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>608</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>모성보호,유연근로,일가정양립</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>고용노동부_사업체노동력조사</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>사업체의 종사자수, 빈 일자리, 노동이동, 근로시간, 임금 등에 관한 사항을 정기적으로 조사하여 산업 유형별 고용상황과 근로시간, 임금상승률 등에 관한 지표를 제공</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/3038232/fileData.do</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>2023-03-31</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>4879</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>1836</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>근로자수,빈일자리수,임금</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>고용노동부_신규화학물질</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>고용노동부가 공표한 신규화학물질의 명칭, 유해성, 제조 수입량, 위험성 정보, 근로자 건강장해 예방을 위한 조치사항 제공</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15002450/fileData.do</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>2023-04-13</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>3480</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>1414</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>화학물질,유해성,위험성</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>고용노동부_근로자 건강센터 현황</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>보건관리가 취약한 소규모 사업장 근로자의 직업병예방 및 건강증진을 위한 기초 직업건강서비스를 제공하기 위해 설치한 근로자 건강센터 설치현황</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15002433/fileData.do</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>2023-04-06</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>3056</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>943</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>건강센터,건강지원센터,센터</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>고용노동부_건설재해예방전문지도기관</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>고용노동부가 공표한 건설재해예방전문지도기관 명단으로 지도기관명, 주소, 전화번호, 관할 지방관서, 지도분야 등에 대한 정보를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15113114/fileData.do</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>2023-04-06</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>건설안전,기술지도,건설재해예방</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>고용노동부_일가정양립실태조사 보고서</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>매년 한국여성정책연구원에 연구용역을 의뢰하여 작성한 연구보고서일가정 양립을 위한 모성보호, 유연근로 실태 현황조사에 대한 보고서</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15032836/fileData.do</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>2023-04-04</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>3853</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>608</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>모성보호,유연근로,일가정양립</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>고용노동부_사업체노동력조사</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>사업체의 종사자수, 빈 일자리, 노동이동, 근로시간, 임금 등에 관한 사항을 정기적으로 조사하여 산업 유형별 고용상황과 근로시간, 임금상승률 등에 관한 지표를 제공</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/3038232/fileData.do</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>2023-03-31</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>4879</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>1836</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>근로자수,빈일자리수,임금</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>고용노동부_신규화학물질</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>고용노동부가 공표한 신규화학물질의 명칭, 유해성, 제조 수입량, 위험성 정보, 근로자 건강장해 예방을 위한 조치사항 제공</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15002450/fileData.do</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>2023-04-13</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>3480</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>1414</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>화학물질,유해성,위험성</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>고용노동부_근로자 건강센터 현황</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>보건관리가 취약한 소규모 사업장 근로자의 직업병예방 및 건강증진을 위한 기초 직업건강서비스를 제공하기 위해 설치한 근로자 건강센터 설치현황</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15002433/fileData.do</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>2023-04-06</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>3056</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>943</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>건강센터,건강지원센터,센터</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>고용노동부_건설재해예방전문지도기관</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>고용노동부가 공표한 건설재해예방전문지도기관 명단으로 지도기관명, 주소, 전화번호, 관할 지방관서, 지도분야 등에 대한 정보를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15113114/fileData.do</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>2023-04-06</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>건설안전,기술지도,건설재해예방</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>고용노동부_일가정양립실태조사 보고서</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>매년 한국여성정책연구원에 연구용역을 의뢰하여 작성한 연구보고서일가정 양립을 위한 모성보호, 유연근로 실태 현황조사에 대한 보고서</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15032836/fileData.do</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>2023-04-04</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>3853</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>608</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>모성보호,유연근로,일가정양립</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>고용노동부_사업체노동력조사</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>사업체의 종사자수, 빈 일자리, 노동이동, 근로시간, 임금 등에 관한 사항을 정기적으로 조사하여 산업 유형별 고용상황과 근로시간, 임금상승률 등에 관한 지표를 제공</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/3038232/fileData.do</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>2023-03-31</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>4879</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>1836</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>근로자수,빈일자리수,임금</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>고용노동부_신규화학물질</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>고용노동부가 공표한 신규화학물질의 명칭, 유해성, 제조 수입량, 위험성 정보, 근로자 건강장해 예방을 위한 조치사항 제공</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15002450/fileData.do</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>2023-04-13</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>3480</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>1414</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>화학물질,유해성,위험성</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>고용노동부_근로자 건강센터 현황</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>보건관리가 취약한 소규모 사업장 근로자의 직업병예방 및 건강증진을 위한 기초 직업건강서비스를 제공하기 위해 설치한 근로자 건강센터 설치현황</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15002433/fileData.do</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>2023-04-06</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>3056</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>943</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>건강센터,건강지원센터,센터</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>고용노동부_건설재해예방전문지도기관</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>고용노동부가 공표한 건설재해예방전문지도기관 명단으로 지도기관명, 주소, 전화번호, 관할 지방관서, 지도분야 등에 대한 정보를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15113114/fileData.do</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>2023-04-06</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>건설안전,기술지도,건설재해예방</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>고용노동부_일가정양립실태조사 보고서</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>매년 한국여성정책연구원에 연구용역을 의뢰하여 작성한 연구보고서일가정 양립을 위한 모성보호, 유연근로 실태 현황조사에 대한 보고서</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15032836/fileData.do</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>2023-04-04</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>3853</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>608</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>모성보호,유연근로,일가정양립</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>고용노동부_사업체노동력조사</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>사업체의 종사자수, 빈 일자리, 노동이동, 근로시간, 임금 등에 관한 사항을 정기적으로 조사하여 산업 유형별 고용상황과 근로시간, 임금상승률 등에 관한 지표를 제공</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/3038232/fileData.do</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>2023-03-31</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>4879</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>1836</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>근로자수,빈일자리수,임금</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>고용노동부_신규화학물질</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>고용노동부가 공표한 신규화학물질의 명칭, 유해성, 제조 수입량, 위험성 정보, 근로자 건강장해 예방을 위한 조치사항 제공</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15002450/fileData.do</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>2023-04-13</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>3480</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>1414</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>화학물질,유해성,위험성</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>고용노동부_근로자 건강센터 현황</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>보건관리가 취약한 소규모 사업장 근로자의 직업병예방 및 건강증진을 위한 기초 직업건강서비스를 제공하기 위해 설치한 근로자 건강센터 설치현황</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15002433/fileData.do</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>2023-04-06</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>3056</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>943</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>건강센터,건강지원센터,센터</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>고용노동부_건설재해예방전문지도기관</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>고용노동부가 공표한 건설재해예방전문지도기관 명단으로 지도기관명, 주소, 전화번호, 관할 지방관서, 지도분야 등에 대한 정보를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15113114/fileData.do</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>2023-04-06</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>건설안전,기술지도,건설재해예방</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>고용노동부_일가정양립실태조사 보고서</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>매년 한국여성정책연구원에 연구용역을 의뢰하여 작성한 연구보고서일가정 양립을 위한 모성보호, 유연근로 실태 현황조사에 대한 보고서</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15032836/fileData.do</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>2023-04-04</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>3853</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>608</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>모성보호,유연근로,일가정양립</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>고용노동부_사업체노동력조사</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>사업체의 종사자수, 빈 일자리, 노동이동, 근로시간, 임금 등에 관한 사항을 정기적으로 조사하여 산업 유형별 고용상황과 근로시간, 임금상승률 등에 관한 지표를 제공</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/3038232/fileData.do</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>2023-03-31</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>4879</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>1836</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>근로자수,빈일자리수,임금</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>고용노동부_신규화학물질</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>고용노동부가 공표한 신규화학물질의 명칭, 유해성, 제조 수입량, 위험성 정보, 근로자 건강장해 예방을 위한 조치사항 제공</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15002450/fileData.do</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>2023-04-13</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>3480</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>1414</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>화학물질,유해성,위험성</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>고용노동부_근로자 건강센터 현황</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>보건관리가 취약한 소규모 사업장 근로자의 직업병예방 및 건강증진을 위한 기초 직업건강서비스를 제공하기 위해 설치한 근로자 건강센터 설치현황</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15002433/fileData.do</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>2023-04-06</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>3056</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>943</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>건강센터,건강지원센터,센터</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>고용노동부_건설재해예방전문지도기관</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>고용노동부가 공표한 건설재해예방전문지도기관 명단으로 지도기관명, 주소, 전화번호, 관할 지방관서, 지도분야 등에 대한 정보를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15113114/fileData.do</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>2023-04-06</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>건설안전,기술지도,건설재해예방</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>고용노동부_일가정양립실태조사 보고서</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>매년 한국여성정책연구원에 연구용역을 의뢰하여 작성한 연구보고서일가정 양립을 위한 모성보호, 유연근로 실태 현황조사에 대한 보고서</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15032836/fileData.do</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>2023-04-04</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>3853</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>608</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>모성보호,유연근로,일가정양립</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>고용노동부_사업체노동력조사</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>사업체의 종사자수, 빈 일자리, 노동이동, 근로시간, 임금 등에 관한 사항을 정기적으로 조사하여 산업 유형별 고용상황과 근로시간, 임금상승률 등에 관한 지표를 제공</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/3038232/fileData.do</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>2023-03-31</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>4879</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>1836</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>근로자수,빈일자리수,임금</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>고용노동부_신규화학물질</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>고용노동부가 공표한 신규화학물질의 명칭, 유해성, 제조 수입량, 위험성 정보, 근로자 건강장해 예방을 위한 조치사항 제공</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15002450/fileData.do</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>2023-04-13</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>3480</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>1414</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>화학물질,유해성,위험성</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>고용노동부_근로자 건강센터 현황</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>보건관리가 취약한 소규모 사업장 근로자의 직업병예방 및 건강증진을 위한 기초 직업건강서비스를 제공하기 위해 설치한 근로자 건강센터 설치현황</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15002433/fileData.do</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>2023-04-06</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>3056</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>943</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>건강센터,건강지원센터,센터</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>고용노동부_건설재해예방전문지도기관</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>고용노동부가 공표한 건설재해예방전문지도기관 명단으로 지도기관명, 주소, 전화번호, 관할 지방관서, 지도분야 등에 대한 정보를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15113114/fileData.do</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>2023-04-06</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>건설안전,기술지도,건설재해예방</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>고용노동부_일가정양립실태조사 보고서</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>매년 한국여성정책연구원에 연구용역을 의뢰하여 작성한 연구보고서일가정 양립을 위한 모성보호, 유연근로 실태 현황조사에 대한 보고서</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15032836/fileData.do</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>2023-04-04</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>3853</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>608</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>모성보호,유연근로,일가정양립</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>고용노동부_사업체노동력조사</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>사업체의 종사자수, 빈 일자리, 노동이동, 근로시간, 임금 등에 관한 사항을 정기적으로 조사하여 산업 유형별 고용상황과 근로시간, 임금상승률 등에 관한 지표를 제공</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/3038232/fileData.do</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>2023-03-31</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>4879</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>1836</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>근로자수,빈일자리수,임금</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>고용노동부_신규화학물질</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>고용노동부가 공표한 신규화학물질의 명칭, 유해성, 제조 수입량, 위험성 정보, 근로자 건강장해 예방을 위한 조치사항 제공</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15002450/fileData.do</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>2023-04-13</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>3480</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>1414</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>화학물질,유해성,위험성</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>고용노동부_근로자 건강센터 현황</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>보건관리가 취약한 소규모 사업장 근로자의 직업병예방 및 건강증진을 위한 기초 직업건강서비스를 제공하기 위해 설치한 근로자 건강센터 설치현황</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15002433/fileData.do</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>2023-04-06</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>3056</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>943</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>건강센터,건강지원센터,센터</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>고용노동부_건설재해예방전문지도기관</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>고용노동부가 공표한 건설재해예방전문지도기관 명단으로 지도기관명, 주소, 전화번호, 관할 지방관서, 지도분야 등에 대한 정보를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15113114/fileData.do</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>2023-04-06</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>건설안전,기술지도,건설재해예방</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>고용노동부_일가정양립실태조사 보고서</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>매년 한국여성정책연구원에 연구용역을 의뢰하여 작성한 연구보고서일가정 양립을 위한 모성보호, 유연근로 실태 현황조사에 대한 보고서</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15032836/fileData.do</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>2023-04-04</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>3853</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>608</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>모성보호,유연근로,일가정양립</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>고용노동부_사업체노동력조사</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>사업체의 종사자수, 빈 일자리, 노동이동, 근로시간, 임금 등에 관한 사항을 정기적으로 조사하여 산업 유형별 고용상황과 근로시간, 임금상승률 등에 관한 지표를 제공</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/3038232/fileData.do</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>2023-03-31</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>4879</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>1836</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>근로자수,빈일자리수,임금</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>고용노동부_신규화학물질</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>고용노동부가 공표한 신규화학물질의 명칭, 유해성, 제조 수입량, 위험성 정보, 근로자 건강장해 예방을 위한 조치사항 제공</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15002450/fileData.do</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>2023-04-13</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>3480</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>1414</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>화학물질,유해성,위험성</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>고용노동부_근로자 건강센터 현황</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>보건관리가 취약한 소규모 사업장 근로자의 직업병예방 및 건강증진을 위한 기초 직업건강서비스를 제공하기 위해 설치한 근로자 건강센터 설치현황</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15002433/fileData.do</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>2023-04-06</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>3056</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>943</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>건강센터,건강지원센터,센터</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>고용노동부_건설재해예방전문지도기관</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>고용노동부가 공표한 건설재해예방전문지도기관 명단으로 지도기관명, 주소, 전화번호, 관할 지방관서, 지도분야 등에 대한 정보를 제공합니다.</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15113114/fileData.do</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>2023-04-06</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>건설안전,기술지도,건설재해예방</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>고용노동부_일가정양립실태조사 보고서</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>매년 한국여성정책연구원에 연구용역을 의뢰하여 작성한 연구보고서일가정 양립을 위한 모성보호, 유연근로 실태 현황조사에 대한 보고서</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/15032836/fileData.do</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>2023-04-04</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>3853</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>608</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>모성보호,유연근로,일가정양립</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>고용노동부_사업체노동력조사</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>사업체의 종사자수, 빈 일자리, 노동이동, 근로시간, 임금 등에 관한 사항을 정기적으로 조사하여 산업 유형별 고용상황과 근로시간, 임금상승률 등에 관한 지표를 제공</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>https://www.data.go.kr/data/3038232/fileData.do</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>고용노동부</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>2023-03-31</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>4879</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>1836</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="I91" t="inlineStr">
         <is>
           <t>근로자수,빈일자리수,임금</t>
         </is>

</xml_diff>